<commit_message>
Update idea about Social Network
</commit_message>
<xml_diff>
--- a/HopeHunt-Start.xlsx
+++ b/HopeHunt-Start.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="103">
   <si>
     <t>Landing Page</t>
   </si>
@@ -322,6 +322,9 @@
   </si>
   <si>
     <t>Robots Cvshared</t>
+  </si>
+  <si>
+    <t>Social Network</t>
   </si>
 </sst>
 </file>
@@ -700,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,6 +857,14 @@
       </c>
       <c r="E12" t="s">
         <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update cons of Share CV - violate Privacy Policy
</commit_message>
<xml_diff>
--- a/HopeHunt-Start.xlsx
+++ b/HopeHunt-Start.xlsx
@@ -10,12 +10,12 @@
     <sheet name="Ideas" sheetId="1" r:id="rId1"/>
     <sheet name="To do" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211" concurrentCalc="0"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="104">
   <si>
     <t>Landing Page</t>
   </si>
@@ -325,6 +325,9 @@
   </si>
   <si>
     <t>Social Network</t>
+  </si>
+  <si>
+    <t>Tuy nhiên: Có vẻ như việc chia sẻ thông tin này chỉ diễn ra ở Việt Nam thì phải, các nước bạn họ rất chi là kỵ việc này. Vì nó sẽ gây ra một rủi ro về QUYỀN THÔNG TIN CÁ NHÂN bị trôi nổi trên thị trường, phiền nhiều vấn đề.</t>
   </si>
 </sst>
 </file>
@@ -703,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,6 +868,11 @@
       </c>
       <c r="D14" t="s">
         <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="D16" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>